<commit_message>
Pushed targets & Planning
</commit_message>
<xml_diff>
--- a/Documents/Targets&Planning.xlsx
+++ b/Documents/Targets&Planning.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BloggingRepositories\blogPosts\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326A31FA-2937-41D7-8E52-17FF7FBF9CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA77F71-DA00-49FC-A95B-3068188EB0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="15196" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
+    <sheet name="Backlogs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,19 +26,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Build a Gallery &amp; Lighthouse feature for vehicleMasti</t>
-  </si>
-  <si>
-    <t>Make loading page for both websites.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>Targets</t>
+  </si>
+  <si>
+    <t>Spending Time</t>
+  </si>
+  <si>
+    <t>Developer Comments</t>
+  </si>
+  <si>
+    <t>Do backlink audit</t>
+  </si>
+  <si>
+    <t>2 Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build Backlinks atleast 20 </t>
+  </si>
+  <si>
+    <t>3 Hours</t>
+  </si>
+  <si>
+    <t>Backlogs</t>
+  </si>
+  <si>
+    <t>Build a gallery and lighthouse feature for VehicleMasti</t>
+  </si>
+  <si>
+    <t>Make loading screen for both the websites</t>
+  </si>
+  <si>
+    <t>Make Patel's Website upto date with VehicleMasti Blog</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,13 +76,56 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,10 +140,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -351,35 +443,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B8:D11"/>
+  <dimension ref="B2:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="J2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="E5" s="3">
+        <v>45251</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="I5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="O5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="S5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="O8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C11" t="s">
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+    </row>
+    <row r="10" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="H11" s="5">
+        <v>2</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="O11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.45">
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:M12"/>
+    <mergeCell ref="O11:Q12"/>
+    <mergeCell ref="J2:R3"/>
+    <mergeCell ref="E5:G6"/>
+    <mergeCell ref="I5:M6"/>
+    <mergeCell ref="O5:Q6"/>
+    <mergeCell ref="S5:V6"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:M9"/>
+    <mergeCell ref="O8:Q9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6280AF-F913-4213-90F7-5D60D9FFA09E}">
+  <dimension ref="F2:Y12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+    </row>
+    <row r="3" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+    </row>
+    <row r="5" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F5" s="7">
         <v>1</v>
       </c>
+      <c r="H5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+    </row>
+    <row r="8" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="11" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F11" s="7">
+        <v>3</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:P12"/>
+    <mergeCell ref="H2:P3"/>
+    <mergeCell ref="R2:Y3"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="H5:P6"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:P9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pushed planning dude & daily status
</commit_message>
<xml_diff>
--- a/Documents/Targets&Planning.xlsx
+++ b/Documents/Targets&Planning.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BloggingRepositories\blogPosts\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA77F71-DA00-49FC-A95B-3068188EB0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FAB564-1456-4B40-95F7-C843A652159E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="15196" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
     <sheet name="Backlogs" sheetId="2" r:id="rId2"/>
+    <sheet name="Backlink_Audit" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>November</t>
   </si>
@@ -62,13 +63,31 @@
   </si>
   <si>
     <t>Make Patel's Website upto date with VehicleMasti Blog</t>
+  </si>
+  <si>
+    <t>Backlinks</t>
+  </si>
+  <si>
+    <t>https://www.dofollowwebsite.com/published</t>
+  </si>
+  <si>
+    <t>http://www.spectrumcommunications.ie/nortel-bcm-50450-end-of-life/#comment-236383</t>
+  </si>
+  <si>
+    <t>https://demcra.com/r/business/1146476_Tata_Safari_Facelift_2023_A_Closer_Look_Into_Modern_SUV</t>
+  </si>
+  <si>
+    <t>https://www.truelovetattoos.it/2016/12/26/add-videos-to-blog-posts/#comment-69235</t>
+  </si>
+  <si>
+    <t>smira.org.uk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +102,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -90,12 +116,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -127,6 +147,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -140,16 +166,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -157,11 +177,23 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -445,154 +477,164 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:V12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.45">
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.45">
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.45">
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>45251</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="I5" s="4" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="I5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="O5" s="4" t="s">
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="O5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="S5" s="4" t="s">
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="S5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.45">
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="H8" s="5">
+      <c r="H8" s="2">
         <v>1</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="O8" s="6" t="s">
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="O8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="11" spans="2:22" x14ac:dyDescent="0.45">
-      <c r="H11" s="5">
+      <c r="H11" s="2">
         <v>2</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="O11" s="6" t="s">
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="O11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.45">
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:M12"/>
-    <mergeCell ref="O11:Q12"/>
-    <mergeCell ref="J2:R3"/>
-    <mergeCell ref="E5:G6"/>
-    <mergeCell ref="I5:M6"/>
-    <mergeCell ref="O5:Q6"/>
     <mergeCell ref="S5:V6"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:M9"/>
     <mergeCell ref="O8:Q9"/>
+    <mergeCell ref="I2:V3"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:M12"/>
+    <mergeCell ref="O11:Q12"/>
+    <mergeCell ref="E5:G6"/>
+    <mergeCell ref="I5:M6"/>
+    <mergeCell ref="O5:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -602,137 +644,137 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6280AF-F913-4213-90F7-5D60D9FFA09E}">
   <dimension ref="F2:Y12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="2" spans="6:25" x14ac:dyDescent="0.45">
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="R2" s="4" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="R2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
     </row>
     <row r="3" spans="6:25" x14ac:dyDescent="0.45">
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
     </row>
     <row r="5" spans="6:25" x14ac:dyDescent="0.45">
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
     </row>
     <row r="6" spans="6:25" x14ac:dyDescent="0.45">
-      <c r="F6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+      <c r="F6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
     </row>
     <row r="8" spans="6:25" x14ac:dyDescent="0.45">
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>2</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
     </row>
     <row r="9" spans="6:25" x14ac:dyDescent="0.45">
-      <c r="F9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="F9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
     </row>
     <row r="11" spans="6:25" x14ac:dyDescent="0.45">
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>3</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
     </row>
     <row r="12" spans="6:25" x14ac:dyDescent="0.45">
-      <c r="F12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
+      <c r="F12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -747,4 +789,107 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E2DAFF-6BFF-4CB8-B294-DE59EA805260}">
+  <dimension ref="C2:P12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="6.53125" customWidth="1"/>
+    <col min="6" max="6" width="9.06640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="J2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+    </row>
+    <row r="3" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="5" spans="3:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C6" s="9"/>
+      <c r="F6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C7" s="9"/>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C8" s="9"/>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C12" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="J2:P3"/>
+    <mergeCell ref="F5:P5"/>
+    <mergeCell ref="F6:P6"/>
+    <mergeCell ref="C5:C12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Planning page & Added 75 day challenge notes
</commit_message>
<xml_diff>
--- a/Documents/Targets&Planning.xlsx
+++ b/Documents/Targets&Planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogging Website\blogPosts\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BloggingRepositories\blogPosts\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B5EE41-C76C-4573-8E83-151BD68052A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE27DEB-5BD3-4601-9D3C-E7F1586C6670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
   <si>
     <t>November</t>
   </si>
@@ -135,13 +135,49 @@
   </si>
   <si>
     <t>26,November,2023, Sunday</t>
+  </si>
+  <si>
+    <t>27,November,2023, Monday</t>
+  </si>
+  <si>
+    <t>Spend atleast 2 hour on Video Scripts &amp; Editing</t>
+  </si>
+  <si>
+    <t>Spend atleast 2 hour on Article Writing</t>
+  </si>
+  <si>
+    <t>Go to GYM</t>
+  </si>
+  <si>
+    <t>1.5 Hour</t>
+  </si>
+  <si>
+    <t>Daily Routines</t>
+  </si>
+  <si>
+    <t>Build 25 Backlinks For Both Patel's &amp; VehicleMasti Blog</t>
+  </si>
+  <si>
+    <t>Read at least 10 pages from selected books</t>
+  </si>
+  <si>
+    <t>Half-an-Hour</t>
+  </si>
+  <si>
+    <t>Daily Tasks</t>
+  </si>
+  <si>
+    <t>Daily Routine Taks One</t>
+  </si>
+  <si>
+    <t>Day 1 of 75</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,8 +220,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +306,16 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -273,35 +326,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -309,6 +364,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -325,12 +383,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Accent5" xfId="3" builtinId="45"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -609,15 +676,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB66"/>
+  <dimension ref="A1:AB104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E45" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+    <sheetView tabSelected="1" topLeftCell="F77" workbookViewId="0">
+      <selection activeCell="M100" sqref="M100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -647,7 +714,7 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -655,31 +722,31 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -687,29 +754,29 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -739,7 +806,7 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -747,12 +814,12 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
       <c r="L5" s="8" t="s">
         <v>1</v>
       </c>
@@ -777,7 +844,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -785,10 +852,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
@@ -807,7 +874,7 @@
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -837,7 +904,7 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -848,34 +915,34 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <v>1</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="6" t="s">
+      <c r="R8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="3" t="s">
+      <c r="V8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -886,26 +953,26 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
       <c r="U9" s="1"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -935,7 +1002,7 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -946,34 +1013,34 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <v>2</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="6" t="s">
+      <c r="R11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="3" t="s">
+      <c r="V11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -984,26 +1051,26 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
       <c r="U12" s="1"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1033,7 +1100,7 @@
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1041,12 +1108,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
       <c r="L14" s="8" t="s">
         <v>1</v>
       </c>
@@ -1071,7 +1138,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1079,10 +1146,10 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
@@ -1101,7 +1168,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1131,7 +1198,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1142,34 +1209,34 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="4">
+      <c r="K17" s="3">
         <v>1</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="L17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="6" t="s">
+      <c r="R17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
       <c r="U17" s="1"/>
-      <c r="V17" s="3" t="s">
+      <c r="V17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1180,26 +1247,26 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
       <c r="U18" s="1"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1229,7 +1296,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1240,34 +1307,34 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="4">
+      <c r="K20" s="3">
         <v>2</v>
       </c>
-      <c r="L20" s="6" t="s">
+      <c r="L20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="6" t="s">
+      <c r="R20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
       <c r="U20" s="1"/>
-      <c r="V20" s="3" t="s">
+      <c r="V20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1278,26 +1345,26 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
       <c r="U21" s="1"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1327,7 +1394,7 @@
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1338,22 +1405,22 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
-      <c r="K23" s="4">
+      <c r="K23" s="3">
         <v>3</v>
       </c>
-      <c r="L23" s="6" t="s">
+      <c r="L23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="6" t="s">
+      <c r="R23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
       <c r="U23" s="1"/>
       <c r="V23" s="10" t="s">
         <v>23</v>
@@ -1365,7 +1432,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1376,16 +1443,16 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="6"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
       <c r="U24" s="1"/>
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
@@ -1395,7 +1462,7 @@
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1425,7 +1492,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
     </row>
-    <row r="26" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1436,7 +1503,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="4">
+      <c r="K26" s="3">
         <v>4</v>
       </c>
       <c r="L26" s="5" t="s">
@@ -1447,11 +1514,11 @@
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="6" t="s">
+      <c r="R26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
       <c r="U26" s="1"/>
       <c r="V26" s="10" t="s">
         <v>23</v>
@@ -1463,7 +1530,7 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1474,16 +1541,16 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-      <c r="K27" s="4"/>
+      <c r="K27" s="3"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
       <c r="U27" s="1"/>
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
@@ -1493,7 +1560,7 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1523,7 +1590,7 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1534,7 +1601,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="4">
+      <c r="K29" s="3">
         <v>5</v>
       </c>
       <c r="L29" s="5" t="s">
@@ -1545,11 +1612,11 @@
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="6" t="s">
+      <c r="R29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
       <c r="U29" s="1"/>
       <c r="V29" s="10" t="s">
         <v>23</v>
@@ -1561,7 +1628,7 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1572,16 +1639,16 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="4"/>
+      <c r="K30" s="3"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="1"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
       <c r="U30" s="1"/>
       <c r="V30" s="10"/>
       <c r="W30" s="10"/>
@@ -1591,7 +1658,7 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1621,7 +1688,7 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
     </row>
-    <row r="32" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1632,7 +1699,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="4">
+      <c r="K32" s="3">
         <v>6</v>
       </c>
       <c r="L32" s="5" t="s">
@@ -1643,23 +1710,23 @@
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="1"/>
-      <c r="R32" s="6" t="s">
+      <c r="R32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S32" s="6"/>
-      <c r="T32" s="6"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
       <c r="U32" s="1"/>
-      <c r="V32" s="3" t="s">
+      <c r="V32" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W32" s="3"/>
-      <c r="X32" s="3"/>
-      <c r="Y32" s="3"/>
-      <c r="Z32" s="3"/>
+      <c r="W32" s="6"/>
+      <c r="X32" s="6"/>
+      <c r="Y32" s="6"/>
+      <c r="Z32" s="6"/>
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1670,26 +1737,26 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="4"/>
+      <c r="K33" s="3"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="1"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="6"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
       <c r="U33" s="1"/>
-      <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
-      <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
-      <c r="Z33" s="3"/>
+      <c r="V33" s="6"/>
+      <c r="W33" s="6"/>
+      <c r="X33" s="6"/>
+      <c r="Y33" s="6"/>
+      <c r="Z33" s="6"/>
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1719,7 +1786,7 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
     </row>
-    <row r="35" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1730,7 +1797,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
-      <c r="K35" s="4">
+      <c r="K35" s="3">
         <v>7</v>
       </c>
       <c r="L35" s="5" t="s">
@@ -1741,11 +1808,11 @@
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="1"/>
-      <c r="R35" s="6" t="s">
+      <c r="R35" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="S35" s="6"/>
-      <c r="T35" s="6"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
       <c r="U35" s="1"/>
       <c r="V35" s="11" t="s">
         <v>28</v>
@@ -1757,7 +1824,7 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1768,16 +1835,16 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
-      <c r="K36" s="4"/>
+      <c r="K36" s="3"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
       <c r="Q36" s="1"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
       <c r="U36" s="1"/>
       <c r="V36" s="11"/>
       <c r="W36" s="11"/>
@@ -1787,7 +1854,7 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1817,7 +1884,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1825,12 +1892,12 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="7" t="s">
+      <c r="H38" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
       <c r="L38" s="8" t="s">
         <v>1</v>
       </c>
@@ -1855,7 +1922,7 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1863,10 +1930,10 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
@@ -1885,7 +1952,7 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1915,7 +1982,7 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1926,34 +1993,34 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="4">
+      <c r="K41" s="3">
         <v>1</v>
       </c>
-      <c r="L41" s="6" t="s">
+      <c r="L41" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
       <c r="Q41" s="1"/>
-      <c r="R41" s="6" t="s">
+      <c r="R41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S41" s="6"/>
-      <c r="T41" s="6"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
       <c r="U41" s="1"/>
-      <c r="V41" s="3" t="s">
+      <c r="V41" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W41" s="3"/>
-      <c r="X41" s="3"/>
-      <c r="Y41" s="3"/>
-      <c r="Z41" s="3"/>
+      <c r="W41" s="6"/>
+      <c r="X41" s="6"/>
+      <c r="Y41" s="6"/>
+      <c r="Z41" s="6"/>
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1964,26 +2031,26 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
       <c r="Q42" s="1"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="6"/>
-      <c r="T42" s="6"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
       <c r="U42" s="1"/>
-      <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
-      <c r="X42" s="3"/>
-      <c r="Y42" s="3"/>
-      <c r="Z42" s="3"/>
+      <c r="V42" s="6"/>
+      <c r="W42" s="6"/>
+      <c r="X42" s="6"/>
+      <c r="Y42" s="6"/>
+      <c r="Z42" s="6"/>
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2013,7 +2080,7 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2024,34 +2091,34 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
-      <c r="K44" s="4">
+      <c r="K44" s="3">
         <v>2</v>
       </c>
-      <c r="L44" s="6" t="s">
+      <c r="L44" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
       <c r="Q44" s="1"/>
-      <c r="R44" s="6" t="s">
+      <c r="R44" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S44" s="6"/>
-      <c r="T44" s="6"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
       <c r="U44" s="1"/>
-      <c r="V44" s="3" t="s">
+      <c r="V44" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W44" s="3"/>
-      <c r="X44" s="3"/>
-      <c r="Y44" s="3"/>
-      <c r="Z44" s="3"/>
+      <c r="W44" s="6"/>
+      <c r="X44" s="6"/>
+      <c r="Y44" s="6"/>
+      <c r="Z44" s="6"/>
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2062,26 +2129,26 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
       <c r="Q45" s="1"/>
-      <c r="R45" s="6"/>
-      <c r="S45" s="6"/>
-      <c r="T45" s="6"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
       <c r="U45" s="1"/>
-      <c r="V45" s="3"/>
-      <c r="W45" s="3"/>
-      <c r="X45" s="3"/>
-      <c r="Y45" s="3"/>
-      <c r="Z45" s="3"/>
+      <c r="V45" s="6"/>
+      <c r="W45" s="6"/>
+      <c r="X45" s="6"/>
+      <c r="Y45" s="6"/>
+      <c r="Z45" s="6"/>
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2111,7 +2178,7 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2122,7 +2189,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
-      <c r="K47" s="4">
+      <c r="K47" s="3">
         <v>3</v>
       </c>
       <c r="L47" s="5" t="s">
@@ -2133,23 +2200,23 @@
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
       <c r="Q47" s="1"/>
-      <c r="R47" s="6" t="s">
+      <c r="R47" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S47" s="6"/>
-      <c r="T47" s="6"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
       <c r="U47" s="1"/>
-      <c r="V47" s="3" t="s">
+      <c r="V47" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W47" s="3"/>
-      <c r="X47" s="3"/>
-      <c r="Y47" s="3"/>
-      <c r="Z47" s="3"/>
+      <c r="W47" s="6"/>
+      <c r="X47" s="6"/>
+      <c r="Y47" s="6"/>
+      <c r="Z47" s="6"/>
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2160,26 +2227,26 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="4"/>
+      <c r="K48" s="3"/>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
       <c r="Q48" s="1"/>
-      <c r="R48" s="6"/>
-      <c r="S48" s="6"/>
-      <c r="T48" s="6"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
       <c r="U48" s="1"/>
-      <c r="V48" s="3"/>
-      <c r="W48" s="3"/>
-      <c r="X48" s="3"/>
-      <c r="Y48" s="3"/>
-      <c r="Z48" s="3"/>
+      <c r="V48" s="6"/>
+      <c r="W48" s="6"/>
+      <c r="X48" s="6"/>
+      <c r="Y48" s="6"/>
+      <c r="Z48" s="6"/>
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2209,7 +2276,7 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
     </row>
-    <row r="50" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2220,7 +2287,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
-      <c r="K50" s="4">
+      <c r="K50" s="3">
         <v>4</v>
       </c>
       <c r="L50" s="5" t="s">
@@ -2231,23 +2298,23 @@
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
       <c r="Q50" s="1"/>
-      <c r="R50" s="6" t="s">
+      <c r="R50" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S50" s="6"/>
-      <c r="T50" s="6"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
       <c r="U50" s="1"/>
-      <c r="V50" s="3" t="s">
+      <c r="V50" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W50" s="3"/>
-      <c r="X50" s="3"/>
-      <c r="Y50" s="3"/>
-      <c r="Z50" s="3"/>
+      <c r="W50" s="6"/>
+      <c r="X50" s="6"/>
+      <c r="Y50" s="6"/>
+      <c r="Z50" s="6"/>
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2258,26 +2325,26 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="4"/>
+      <c r="K51" s="3"/>
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
       <c r="Q51" s="1"/>
-      <c r="R51" s="6"/>
-      <c r="S51" s="6"/>
-      <c r="T51" s="6"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
       <c r="U51" s="1"/>
-      <c r="V51" s="3"/>
-      <c r="W51" s="3"/>
-      <c r="X51" s="3"/>
-      <c r="Y51" s="3"/>
-      <c r="Z51" s="3"/>
+      <c r="V51" s="6"/>
+      <c r="W51" s="6"/>
+      <c r="X51" s="6"/>
+      <c r="Y51" s="6"/>
+      <c r="Z51" s="6"/>
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2307,7 +2374,7 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2315,12 +2382,12 @@
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="7" t="s">
+      <c r="H53" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
       <c r="L53" s="8" t="s">
         <v>1</v>
       </c>
@@ -2345,11 +2412,11 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
       <c r="N54" s="8"/>
@@ -2366,57 +2433,57 @@
       <c r="Y54" s="8"/>
       <c r="Z54" s="8"/>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H56" s="17" t="s">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="H56" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I56" s="17"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17"/>
-      <c r="O56" s="17"/>
-      <c r="P56" s="17"/>
-      <c r="Q56" s="17"/>
-      <c r="R56" s="17"/>
-      <c r="S56" s="17"/>
-      <c r="T56" s="17"/>
-      <c r="U56" s="17"/>
-      <c r="V56" s="17"/>
-      <c r="W56" s="17"/>
-      <c r="X56" s="17"/>
-      <c r="Y56" s="17"/>
-      <c r="Z56" s="17"/>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H57" s="17"/>
-      <c r="I57" s="17"/>
-      <c r="J57" s="17"/>
-      <c r="K57" s="17"/>
-      <c r="L57" s="17"/>
-      <c r="M57" s="17"/>
-      <c r="N57" s="17"/>
-      <c r="O57" s="17"/>
-      <c r="P57" s="17"/>
-      <c r="Q57" s="17"/>
-      <c r="R57" s="17"/>
-      <c r="S57" s="17"/>
-      <c r="T57" s="17"/>
-      <c r="U57" s="17"/>
-      <c r="V57" s="17"/>
-      <c r="W57" s="17"/>
-      <c r="X57" s="17"/>
-      <c r="Y57" s="17"/>
-      <c r="Z57" s="17"/>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H59" s="7" t="s">
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12"/>
+      <c r="N56" s="12"/>
+      <c r="O56" s="12"/>
+      <c r="P56" s="12"/>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="12"/>
+      <c r="S56" s="12"/>
+      <c r="T56" s="12"/>
+      <c r="U56" s="12"/>
+      <c r="V56" s="12"/>
+      <c r="W56" s="12"/>
+      <c r="X56" s="12"/>
+      <c r="Y56" s="12"/>
+      <c r="Z56" s="12"/>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="12"/>
+      <c r="M57" s="12"/>
+      <c r="N57" s="12"/>
+      <c r="O57" s="12"/>
+      <c r="P57" s="12"/>
+      <c r="Q57" s="12"/>
+      <c r="R57" s="12"/>
+      <c r="S57" s="12"/>
+      <c r="T57" s="12"/>
+      <c r="U57" s="12"/>
+      <c r="V57" s="12"/>
+      <c r="W57" s="12"/>
+      <c r="X57" s="12"/>
+      <c r="Y57" s="12"/>
+      <c r="Z57" s="12"/>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="H59" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
       <c r="L59" s="8" t="s">
         <v>1</v>
       </c>
@@ -2439,11 +2506,11 @@
       <c r="Y59" s="8"/>
       <c r="Z59" s="8"/>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
       <c r="L60" s="8"/>
       <c r="M60" s="8"/>
       <c r="N60" s="8"/>
@@ -2460,57 +2527,57 @@
       <c r="Y60" s="8"/>
       <c r="Z60" s="8"/>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H62" s="17" t="s">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="H62" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I62" s="17"/>
-      <c r="J62" s="17"/>
-      <c r="K62" s="17"/>
-      <c r="L62" s="17"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="17"/>
-      <c r="O62" s="17"/>
-      <c r="P62" s="17"/>
-      <c r="Q62" s="17"/>
-      <c r="R62" s="17"/>
-      <c r="S62" s="17"/>
-      <c r="T62" s="17"/>
-      <c r="U62" s="17"/>
-      <c r="V62" s="17"/>
-      <c r="W62" s="17"/>
-      <c r="X62" s="17"/>
-      <c r="Y62" s="17"/>
-      <c r="Z62" s="17"/>
-    </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="H63" s="17"/>
-      <c r="I63" s="17"/>
-      <c r="J63" s="17"/>
-      <c r="K63" s="17"/>
-      <c r="L63" s="17"/>
-      <c r="M63" s="17"/>
-      <c r="N63" s="17"/>
-      <c r="O63" s="17"/>
-      <c r="P63" s="17"/>
-      <c r="Q63" s="17"/>
-      <c r="R63" s="17"/>
-      <c r="S63" s="17"/>
-      <c r="T63" s="17"/>
-      <c r="U63" s="17"/>
-      <c r="V63" s="17"/>
-      <c r="W63" s="17"/>
-      <c r="X63" s="17"/>
-      <c r="Y63" s="17"/>
-      <c r="Z63" s="17"/>
-    </row>
-    <row r="65" spans="8:26" x14ac:dyDescent="0.25">
-      <c r="H65" s="7" t="s">
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="12"/>
+      <c r="P62" s="12"/>
+      <c r="Q62" s="12"/>
+      <c r="R62" s="12"/>
+      <c r="S62" s="12"/>
+      <c r="T62" s="12"/>
+      <c r="U62" s="12"/>
+      <c r="V62" s="12"/>
+      <c r="W62" s="12"/>
+      <c r="X62" s="12"/>
+      <c r="Y62" s="12"/>
+      <c r="Z62" s="12"/>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
+      <c r="L63" s="12"/>
+      <c r="M63" s="12"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="12"/>
+      <c r="P63" s="12"/>
+      <c r="Q63" s="12"/>
+      <c r="R63" s="12"/>
+      <c r="S63" s="12"/>
+      <c r="T63" s="12"/>
+      <c r="U63" s="12"/>
+      <c r="V63" s="12"/>
+      <c r="W63" s="12"/>
+      <c r="X63" s="12"/>
+      <c r="Y63" s="12"/>
+      <c r="Z63" s="12"/>
+    </row>
+    <row r="65" spans="8:26" x14ac:dyDescent="0.45">
+      <c r="H65" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I65" s="7"/>
-      <c r="J65" s="7"/>
-      <c r="K65" s="7"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
       <c r="L65" s="8" t="s">
         <v>1</v>
       </c>
@@ -2533,11 +2600,11 @@
       <c r="Y65" s="8"/>
       <c r="Z65" s="8"/>
     </row>
-    <row r="66" spans="8:26" x14ac:dyDescent="0.25">
-      <c r="H66" s="7"/>
-      <c r="I66" s="7"/>
-      <c r="J66" s="7"/>
-      <c r="K66" s="7"/>
+    <row r="66" spans="8:26" x14ac:dyDescent="0.45">
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
       <c r="L66" s="8"/>
       <c r="M66" s="8"/>
       <c r="N66" s="8"/>
@@ -2554,8 +2621,445 @@
       <c r="Y66" s="8"/>
       <c r="Z66" s="8"/>
     </row>
+    <row r="68" spans="8:26" x14ac:dyDescent="0.45">
+      <c r="H68" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I68" s="12"/>
+      <c r="J68" s="12"/>
+      <c r="K68" s="12"/>
+      <c r="L68" s="12"/>
+      <c r="M68" s="12"/>
+      <c r="N68" s="12"/>
+      <c r="O68" s="12"/>
+      <c r="P68" s="12"/>
+      <c r="Q68" s="12"/>
+      <c r="R68" s="12"/>
+      <c r="S68" s="12"/>
+      <c r="T68" s="12"/>
+      <c r="U68" s="12"/>
+      <c r="V68" s="12"/>
+      <c r="W68" s="12"/>
+      <c r="X68" s="12"/>
+      <c r="Y68" s="12"/>
+      <c r="Z68" s="12"/>
+    </row>
+    <row r="69" spans="8:26" x14ac:dyDescent="0.45">
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
+      <c r="L69" s="12"/>
+      <c r="M69" s="12"/>
+      <c r="N69" s="12"/>
+      <c r="O69" s="12"/>
+      <c r="P69" s="12"/>
+      <c r="Q69" s="12"/>
+      <c r="R69" s="12"/>
+      <c r="S69" s="12"/>
+      <c r="T69" s="12"/>
+      <c r="U69" s="12"/>
+      <c r="V69" s="12"/>
+      <c r="W69" s="12"/>
+      <c r="X69" s="12"/>
+      <c r="Y69" s="12"/>
+      <c r="Z69" s="12"/>
+    </row>
+    <row r="71" spans="8:26" x14ac:dyDescent="0.45">
+      <c r="H71" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M71" s="8"/>
+      <c r="N71" s="8"/>
+      <c r="O71" s="8"/>
+      <c r="P71" s="8"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S71" s="8"/>
+      <c r="T71" s="8"/>
+      <c r="U71" s="1"/>
+      <c r="V71" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="W71" s="8"/>
+      <c r="X71" s="8"/>
+      <c r="Y71" s="8"/>
+      <c r="Z71" s="8"/>
+    </row>
+    <row r="72" spans="8:26" x14ac:dyDescent="0.45">
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="8"/>
+      <c r="M72" s="8"/>
+      <c r="N72" s="8"/>
+      <c r="O72" s="8"/>
+      <c r="P72" s="8"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="8"/>
+      <c r="S72" s="8"/>
+      <c r="T72" s="8"/>
+      <c r="U72" s="1"/>
+      <c r="V72" s="8"/>
+      <c r="W72" s="8"/>
+      <c r="X72" s="8"/>
+      <c r="Y72" s="8"/>
+      <c r="Z72" s="8"/>
+    </row>
+    <row r="73" spans="8:26" x14ac:dyDescent="0.45">
+      <c r="N73" s="18"/>
+      <c r="O73" s="18"/>
+      <c r="P73" s="18"/>
+      <c r="Q73" s="18"/>
+      <c r="R73" s="18"/>
+      <c r="S73" s="18"/>
+      <c r="T73" s="18"/>
+      <c r="U73" s="18"/>
+      <c r="V73" s="18"/>
+      <c r="W73" s="18"/>
+      <c r="X73" s="18"/>
+      <c r="Y73" s="18"/>
+      <c r="Z73" s="18"/>
+    </row>
+    <row r="75" spans="8:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I75" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K75" s="3">
+        <v>1</v>
+      </c>
+      <c r="L75" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
+      <c r="O75" s="5"/>
+      <c r="P75" s="5"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S75" s="4"/>
+      <c r="T75" s="4"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="18"/>
+      <c r="W75" s="18"/>
+      <c r="X75" s="18"/>
+      <c r="Y75" s="18"/>
+      <c r="Z75" s="18"/>
+    </row>
+    <row r="76" spans="8:26" x14ac:dyDescent="0.45">
+      <c r="I76" s="20"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+      <c r="O76" s="5"/>
+      <c r="P76" s="5"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="4"/>
+      <c r="S76" s="4"/>
+      <c r="T76" s="4"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="18"/>
+      <c r="W76" s="18"/>
+      <c r="X76" s="18"/>
+      <c r="Y76" s="18"/>
+      <c r="Z76" s="18"/>
+    </row>
+    <row r="77" spans="8:26" x14ac:dyDescent="0.45">
+      <c r="I77" s="20"/>
+    </row>
+    <row r="78" spans="8:26" x14ac:dyDescent="0.45">
+      <c r="I78" s="20"/>
+      <c r="K78" s="3">
+        <v>2</v>
+      </c>
+      <c r="L78" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="4"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S78" s="4"/>
+      <c r="T78" s="4"/>
+      <c r="U78" s="1"/>
+      <c r="V78" s="18"/>
+      <c r="W78" s="18"/>
+      <c r="X78" s="18"/>
+      <c r="Y78" s="18"/>
+      <c r="Z78" s="18"/>
+    </row>
+    <row r="79" spans="8:26" x14ac:dyDescent="0.45">
+      <c r="I79" s="20"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="4"/>
+      <c r="N79" s="4"/>
+      <c r="O79" s="4"/>
+      <c r="P79" s="4"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="4"/>
+      <c r="S79" s="4"/>
+      <c r="T79" s="4"/>
+      <c r="U79" s="1"/>
+      <c r="V79" s="18"/>
+      <c r="W79" s="18"/>
+      <c r="X79" s="18"/>
+      <c r="Y79" s="18"/>
+      <c r="Z79" s="18"/>
+    </row>
+    <row r="80" spans="8:26" x14ac:dyDescent="0.45">
+      <c r="I80" s="20"/>
+    </row>
+    <row r="81" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="I81" s="20"/>
+      <c r="K81" s="3">
+        <v>3</v>
+      </c>
+      <c r="L81" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S81" s="4"/>
+      <c r="T81" s="4"/>
+    </row>
+    <row r="82" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G82" s="21"/>
+      <c r="I82" s="20"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="4"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="4"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="4"/>
+      <c r="S82" s="4"/>
+      <c r="T82" s="4"/>
+    </row>
+    <row r="83" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G83" s="21"/>
+      <c r="I83" s="20"/>
+    </row>
+    <row r="84" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G84" s="21"/>
+      <c r="I84" s="20"/>
+      <c r="K84" s="3">
+        <v>4</v>
+      </c>
+      <c r="L84" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="4"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S84" s="4"/>
+      <c r="T84" s="4"/>
+    </row>
+    <row r="85" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G85" s="21"/>
+      <c r="I85" s="20"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="4"/>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="4"/>
+      <c r="P85" s="4"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="4"/>
+      <c r="S85" s="4"/>
+      <c r="T85" s="4"/>
+    </row>
+    <row r="86" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G86" s="21"/>
+      <c r="I86" s="20"/>
+    </row>
+    <row r="87" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G87" s="21"/>
+      <c r="I87" s="20"/>
+      <c r="K87" s="3">
+        <v>5</v>
+      </c>
+      <c r="L87" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M87" s="4"/>
+      <c r="N87" s="4"/>
+      <c r="O87" s="4"/>
+      <c r="P87" s="4"/>
+      <c r="Q87" s="1"/>
+      <c r="R87" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="S87" s="4"/>
+      <c r="T87" s="4"/>
+    </row>
+    <row r="88" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G88" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I88" s="20"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="4"/>
+      <c r="Q88" s="1"/>
+      <c r="R88" s="4"/>
+      <c r="S88" s="4"/>
+      <c r="T88" s="4"/>
+    </row>
+    <row r="89" spans="7:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G89" s="19"/>
+    </row>
+    <row r="90" spans="7:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G90" s="19"/>
+      <c r="I90" s="18"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="18"/>
+      <c r="M90" s="18"/>
+      <c r="N90" s="18"/>
+      <c r="O90" s="18"/>
+      <c r="P90" s="18"/>
+      <c r="Q90" s="18"/>
+      <c r="R90" s="18"/>
+      <c r="S90" s="18"/>
+      <c r="T90" s="18"/>
+    </row>
+    <row r="91" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G91" s="19"/>
+      <c r="I91" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K91" s="3">
+        <v>1</v>
+      </c>
+      <c r="L91" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M91" s="5"/>
+      <c r="N91" s="5"/>
+      <c r="O91" s="5"/>
+      <c r="P91" s="5"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S91" s="4"/>
+      <c r="T91" s="4"/>
+    </row>
+    <row r="92" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G92" s="21"/>
+      <c r="I92" s="20"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="5"/>
+      <c r="M92" s="5"/>
+      <c r="N92" s="5"/>
+      <c r="O92" s="5"/>
+      <c r="P92" s="5"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="4"/>
+      <c r="S92" s="4"/>
+      <c r="T92" s="4"/>
+    </row>
+    <row r="93" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G93" s="21"/>
+      <c r="I93" s="20"/>
+    </row>
+    <row r="94" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G94" s="21"/>
+      <c r="I94" s="20"/>
+    </row>
+    <row r="95" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G95" s="21"/>
+      <c r="I95" s="20"/>
+    </row>
+    <row r="96" spans="7:20" x14ac:dyDescent="0.45">
+      <c r="G96" s="21"/>
+      <c r="I96" s="20"/>
+    </row>
+    <row r="97" spans="7:9" x14ac:dyDescent="0.45">
+      <c r="G97" s="21"/>
+      <c r="I97" s="20"/>
+    </row>
+    <row r="98" spans="7:9" x14ac:dyDescent="0.45">
+      <c r="G98" s="21"/>
+      <c r="I98" s="20"/>
+    </row>
+    <row r="99" spans="7:9" x14ac:dyDescent="0.45">
+      <c r="I99" s="20"/>
+    </row>
+    <row r="100" spans="7:9" x14ac:dyDescent="0.45">
+      <c r="I100" s="20"/>
+    </row>
+    <row r="101" spans="7:9" x14ac:dyDescent="0.45">
+      <c r="I101" s="20"/>
+    </row>
+    <row r="102" spans="7:9" x14ac:dyDescent="0.45">
+      <c r="I102" s="20"/>
+    </row>
+    <row r="103" spans="7:9" x14ac:dyDescent="0.45">
+      <c r="I103" s="20"/>
+    </row>
+    <row r="104" spans="7:9" x14ac:dyDescent="0.45">
+      <c r="I104" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="79">
+  <mergeCells count="105">
+    <mergeCell ref="G88:G91"/>
+    <mergeCell ref="I91:I104"/>
+    <mergeCell ref="K91:K92"/>
+    <mergeCell ref="L91:P92"/>
+    <mergeCell ref="R91:T92"/>
+    <mergeCell ref="L81:P82"/>
+    <mergeCell ref="R81:T82"/>
+    <mergeCell ref="K84:K85"/>
+    <mergeCell ref="L84:P85"/>
+    <mergeCell ref="R84:T85"/>
+    <mergeCell ref="L78:P79"/>
+    <mergeCell ref="R78:T79"/>
+    <mergeCell ref="K87:K88"/>
+    <mergeCell ref="L87:P88"/>
+    <mergeCell ref="R87:T88"/>
+    <mergeCell ref="I75:I88"/>
+    <mergeCell ref="K78:K79"/>
+    <mergeCell ref="K81:K82"/>
+    <mergeCell ref="K75:K76"/>
+    <mergeCell ref="L75:P76"/>
+    <mergeCell ref="R75:T76"/>
+    <mergeCell ref="H68:Z69"/>
+    <mergeCell ref="H71:K72"/>
+    <mergeCell ref="L71:P72"/>
+    <mergeCell ref="R71:T72"/>
+    <mergeCell ref="V71:Z72"/>
     <mergeCell ref="L65:P66"/>
     <mergeCell ref="R65:T66"/>
     <mergeCell ref="V65:Z66"/>
@@ -2571,17 +3075,28 @@
     <mergeCell ref="R53:T54"/>
     <mergeCell ref="V53:Z54"/>
     <mergeCell ref="V35:Z36"/>
+    <mergeCell ref="L38:P39"/>
+    <mergeCell ref="R38:T39"/>
+    <mergeCell ref="V38:Z39"/>
+    <mergeCell ref="K41:K42"/>
+    <mergeCell ref="L41:P42"/>
+    <mergeCell ref="R41:T42"/>
+    <mergeCell ref="V41:Z42"/>
+    <mergeCell ref="H38:K39"/>
+    <mergeCell ref="V50:Z51"/>
+    <mergeCell ref="V44:Z45"/>
+    <mergeCell ref="K47:K48"/>
+    <mergeCell ref="V29:Z30"/>
+    <mergeCell ref="V32:Z33"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L35:P36"/>
+    <mergeCell ref="R35:T36"/>
     <mergeCell ref="K29:K30"/>
     <mergeCell ref="L29:P30"/>
     <mergeCell ref="R29:T30"/>
     <mergeCell ref="K32:K33"/>
     <mergeCell ref="L32:P33"/>
     <mergeCell ref="R32:T33"/>
-    <mergeCell ref="V29:Z30"/>
-    <mergeCell ref="V32:Z33"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L35:P36"/>
-    <mergeCell ref="R35:T36"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="L23:P24"/>
     <mergeCell ref="R23:T24"/>
@@ -2598,14 +3113,15 @@
     <mergeCell ref="L20:P21"/>
     <mergeCell ref="R20:T21"/>
     <mergeCell ref="V20:Z21"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:P12"/>
-    <mergeCell ref="R11:T12"/>
     <mergeCell ref="V11:Z12"/>
     <mergeCell ref="L14:P15"/>
     <mergeCell ref="R14:T15"/>
     <mergeCell ref="V14:Z15"/>
     <mergeCell ref="H14:K15"/>
+    <mergeCell ref="V47:Z48"/>
+    <mergeCell ref="K50:K51"/>
+    <mergeCell ref="L50:P51"/>
+    <mergeCell ref="R50:T51"/>
     <mergeCell ref="H2:Z3"/>
     <mergeCell ref="R5:T6"/>
     <mergeCell ref="V5:Z6"/>
@@ -2615,26 +3131,14 @@
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="L8:P9"/>
     <mergeCell ref="H5:K6"/>
-    <mergeCell ref="L38:P39"/>
-    <mergeCell ref="R38:T39"/>
-    <mergeCell ref="V38:Z39"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="L41:P42"/>
-    <mergeCell ref="R41:T42"/>
-    <mergeCell ref="V41:Z42"/>
-    <mergeCell ref="H38:K39"/>
-    <mergeCell ref="V50:Z51"/>
-    <mergeCell ref="V44:Z45"/>
-    <mergeCell ref="K47:K48"/>
-    <mergeCell ref="L47:P48"/>
-    <mergeCell ref="R47:T48"/>
-    <mergeCell ref="V47:Z48"/>
-    <mergeCell ref="K50:K51"/>
-    <mergeCell ref="L50:P51"/>
-    <mergeCell ref="R50:T51"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:P12"/>
+    <mergeCell ref="R11:T12"/>
     <mergeCell ref="K44:K45"/>
     <mergeCell ref="L44:P45"/>
     <mergeCell ref="R44:T45"/>
+    <mergeCell ref="L47:P48"/>
+    <mergeCell ref="R47:T48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2648,161 +3152,161 @@
       <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="H2" s="12" t="s">
+    <row r="2" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="H2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="R2" s="12" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="R2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-    </row>
-    <row r="3" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-    </row>
-    <row r="5" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F5" s="13">
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+    </row>
+    <row r="3" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+    </row>
+    <row r="5" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F5" s="14">
         <v>1</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-    </row>
-    <row r="6" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-    </row>
-    <row r="8" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F8" s="13">
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+    </row>
+    <row r="6" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+    </row>
+    <row r="8" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F8" s="14">
         <v>2</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-    </row>
-    <row r="9" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-    </row>
-    <row r="11" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F11" s="13">
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+    </row>
+    <row r="9" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+    </row>
+    <row r="11" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F11" s="14">
         <v>3</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-    </row>
-    <row r="12" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-    </row>
-    <row r="14" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F14" s="13">
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+    </row>
+    <row r="12" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+    </row>
+    <row r="14" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F14" s="14">
         <v>4</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-    </row>
-    <row r="15" spans="6:25" x14ac:dyDescent="0.25">
-      <c r="F15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+    </row>
+    <row r="15" spans="6:25" x14ac:dyDescent="0.45">
+      <c r="F15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2829,89 +3333,89 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.59765625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="J2" s="14" t="s">
+    <row r="2" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="J2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-    </row>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-    </row>
-    <row r="5" spans="3:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="16" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+    </row>
+    <row r="3" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+    </row>
+    <row r="5" spans="3:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C6" s="16"/>
-      <c r="F6" s="15" t="s">
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C6" s="17"/>
+      <c r="F6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C7" s="17"/>
       <c r="F7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="16"/>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C8" s="17"/>
       <c r="F8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C9" s="16"/>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C10" s="16"/>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C11" s="16"/>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="16"/>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.45">
+      <c r="C12" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>